<commit_message>
Update condition Continue engulfing
Improve winrate for XAU, BTC, ETH timeframe H1, H4
</commit_message>
<xml_diff>
--- a/Analysh/Timeframe_Winrate.xlsx
+++ b/Analysh/Timeframe_Winrate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trading\Coding\PriceAction\Analysh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6BAB3D-3FF3-46ED-8D84-CB00BD612D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F396A-2F23-4AD4-BC81-50AEDD32B196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1365" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="202502" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>Version</t>
   </si>
@@ -120,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +146,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9933FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,16 +191,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -198,10 +212,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -489,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I8"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,44 +521,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -565,7 +582,7 @@
       <c r="H4" s="1">
         <v>33.33</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -591,7 +608,7 @@
       <c r="H5" s="1">
         <v>50</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
@@ -603,10 +620,10 @@
       <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>50</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="4">
         <v>48</v>
       </c>
       <c r="G6" s="1">
@@ -615,7 +632,7 @@
       <c r="H6" s="1">
         <v>57.14</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -627,10 +644,10 @@
       <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>89</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="4">
         <v>38</v>
       </c>
       <c r="G7" s="1">
@@ -639,7 +656,7 @@
       <c r="H7" s="1">
         <v>32</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
@@ -657,16 +674,169 @@
       <c r="F8" s="1">
         <v>34.409999999999997</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="5">
         <v>19</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="5">
         <v>47.31</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="12" spans="2:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>20250203</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>20250203</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>20250203</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="11">
+        <v>82</v>
+      </c>
+      <c r="F16" s="11">
+        <v>40.24</v>
+      </c>
+      <c r="G16" s="12">
+        <v>23</v>
+      </c>
+      <c r="H16" s="12">
+        <v>43.48</v>
+      </c>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>20250203</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="11">
+        <v>168</v>
+      </c>
+      <c r="F17" s="11">
+        <v>38.29</v>
+      </c>
+      <c r="G17" s="12">
+        <v>32</v>
+      </c>
+      <c r="H17" s="12">
+        <v>37.5</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1">
+        <v>20250203</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="12">
+        <v>157</v>
+      </c>
+      <c r="F18" s="12">
+        <v>38.85</v>
+      </c>
+      <c r="G18" s="13">
+        <v>38</v>
+      </c>
+      <c r="H18" s="14">
+        <v>44.74</v>
+      </c>
+      <c r="I18" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="I4:I8"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>

</xml_diff>

<commit_message>
20250210_Add new strategy 3 pairs engulfing
get more chance to open position
</commit_message>
<xml_diff>
--- a/Analysh/Timeframe_Winrate.xlsx
+++ b/Analysh/Timeframe_Winrate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trading\Coding\PriceAction\Analysh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F396A-2F23-4AD4-BC81-50AEDD32B196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D042CF6-708C-4483-A63B-42A8DBB32F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="20">
   <si>
     <t>Version</t>
   </si>
@@ -70,13 +70,28 @@
   </si>
   <si>
     <t>2:1</t>
+  </si>
+  <si>
+    <t>USDJPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time backtest </t>
+  </si>
+  <si>
+    <t>20220201 - 20250208</t>
+  </si>
+  <si>
+    <t>With only strategy 1</t>
+  </si>
+  <si>
+    <t>With strategy 1 and strategy 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +134,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +184,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -185,13 +214,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -202,6 +281,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -211,14 +298,28 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -506,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,32 +621,32 @@
     <col min="5" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:16" ht="18" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+    <row r="3" spans="2:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
@@ -558,9 +659,9 @@
       <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -582,11 +683,11 @@
       <c r="H4" s="1">
         <v>33.33</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -608,9 +709,9 @@
       <c r="H5" s="1">
         <v>50</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -632,9 +733,13 @@
       <c r="H6" s="1">
         <v>57.14</v>
       </c>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="12"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+    </row>
+    <row r="7" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -656,9 +761,13 @@
       <c r="H7" s="1">
         <v>32</v>
       </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="12"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+    </row>
+    <row r="8" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -680,34 +789,64 @@
       <c r="H8" s="5">
         <v>47.31</v>
       </c>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="12" spans="2:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B12" s="9" t="s">
+      <c r="I8" s="12"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+    </row>
+    <row r="9" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+    </row>
+    <row r="10" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="M10" s="27"/>
+      <c r="N10" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+    </row>
+    <row r="11" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+    </row>
+    <row r="12" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+    </row>
+    <row r="13" spans="2:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
@@ -720,9 +859,13 @@
       <c r="H13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="11"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -732,15 +875,15 @@
       <c r="D14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="6" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -750,13 +893,13 @@
       <c r="D15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -766,21 +909,21 @@
       <c r="D16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="7">
         <v>82</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="7">
         <v>40.24</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="8">
         <v>23</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="8">
         <v>43.48</v>
       </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
@@ -790,21 +933,21 @@
       <c r="D17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="7">
         <v>168</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="7">
         <v>38.29</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="8">
         <v>32</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="8">
         <v>37.5</v>
       </c>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
@@ -814,22 +957,421 @@
       <c r="D18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="8">
         <v>157</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="8">
         <v>38.85</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="9">
         <v>38</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="10">
         <v>44.74</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="22" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="B22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="15">
+        <v>134</v>
+      </c>
+      <c r="F24" s="15">
+        <v>32.090000000000003</v>
+      </c>
+      <c r="G24" s="15">
+        <v>29</v>
+      </c>
+      <c r="H24" s="17">
+        <v>48.28</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="15">
+        <v>117</v>
+      </c>
+      <c r="F25" s="15">
+        <v>33.33</v>
+      </c>
+      <c r="G25" s="15">
+        <v>26</v>
+      </c>
+      <c r="H25" s="17">
+        <v>30.77</v>
+      </c>
+      <c r="I25" s="20"/>
+    </row>
+    <row r="26" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="22">
+        <v>112</v>
+      </c>
+      <c r="F26" s="22">
+        <v>40.18</v>
+      </c>
+      <c r="G26" s="15">
+        <v>29</v>
+      </c>
+      <c r="H26" s="17">
+        <v>20.69</v>
+      </c>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="23">
+        <v>232</v>
+      </c>
+      <c r="F27" s="23">
+        <v>39.22</v>
+      </c>
+      <c r="G27" s="15">
+        <v>51</v>
+      </c>
+      <c r="H27" s="17">
+        <v>29.41</v>
+      </c>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="22">
+        <v>214</v>
+      </c>
+      <c r="F28" s="22">
+        <v>39.25</v>
+      </c>
+      <c r="G28" s="25">
+        <v>50</v>
+      </c>
+      <c r="H28" s="26">
+        <v>44</v>
+      </c>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="22">
+        <v>119</v>
+      </c>
+      <c r="F29" s="22">
+        <v>39.5</v>
+      </c>
+      <c r="G29" s="22">
+        <v>35</v>
+      </c>
+      <c r="H29" s="24">
+        <v>40</v>
+      </c>
+      <c r="I29" s="21"/>
+    </row>
+    <row r="33" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="14"/>
+      <c r="I33" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="15">
+        <v>263</v>
+      </c>
+      <c r="F35" s="15">
+        <v>33.08</v>
+      </c>
+      <c r="G35" s="15">
+        <v>74</v>
+      </c>
+      <c r="H35" s="17">
+        <v>31.08</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="15">
+        <v>232</v>
+      </c>
+      <c r="F36" s="15">
+        <v>31.03</v>
+      </c>
+      <c r="G36" s="15">
+        <v>68</v>
+      </c>
+      <c r="H36" s="17">
+        <v>25</v>
+      </c>
+      <c r="I36" s="20"/>
+    </row>
+    <row r="37" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="22">
+        <v>234</v>
+      </c>
+      <c r="F37" s="22">
+        <v>39.32</v>
+      </c>
+      <c r="G37" s="15">
+        <v>65</v>
+      </c>
+      <c r="H37" s="17">
+        <v>26.15</v>
+      </c>
+      <c r="I37" s="20"/>
+      <c r="L37" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="16">
+        <v>358</v>
+      </c>
+      <c r="F38" s="16">
+        <v>34.92</v>
+      </c>
+      <c r="G38" s="15">
+        <v>94</v>
+      </c>
+      <c r="H38" s="17">
+        <v>29.79</v>
+      </c>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="22">
+        <v>366</v>
+      </c>
+      <c r="F39" s="22">
+        <v>38.25</v>
+      </c>
+      <c r="G39" s="25">
+        <v>94</v>
+      </c>
+      <c r="H39" s="26">
+        <v>45.74</v>
+      </c>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1">
+        <v>20250209</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="22">
+        <v>261</v>
+      </c>
+      <c r="F40" s="22">
+        <v>39.85</v>
+      </c>
+      <c r="G40" s="15">
+        <v>65</v>
+      </c>
+      <c r="H40" s="17">
+        <v>26.15</v>
+      </c>
+      <c r="I40" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="28">
+    <mergeCell ref="I35:I40"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I29"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I4:I8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="I14:I18"/>
     <mergeCell ref="B12:B13"/>
@@ -837,13 +1379,6 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I4:I8"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>